<commit_message>
Update specs & Booking model idea
</commit_message>
<xml_diff>
--- a/Documents/CitizenTaxi.xlsx
+++ b/Documents/CitizenTaxi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani146d\Documents\GitHub\Techcollege\Education\Module 6\PatientTaxi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani146d\Documents\GitHub\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6449E01D-6047-48CE-8468-65F51D78B7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0FA103-D00E-4BAA-A752-676E003A7C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>Krav Id</t>
   </si>
@@ -312,6 +312,36 @@
   </si>
   <si>
     <t>Citizen CRUD egen booking</t>
+  </si>
+  <si>
+    <t>Borgern bør præsenteres for taxabooking formularen med en side pr. Spørgsmål, så borgeren ikke bliver overbelastet af information</t>
+  </si>
+  <si>
+    <t>Brugeren kan stoppe notifikationer ved hjælp af checkbox efter bookingsprocessen er færdig</t>
+  </si>
+  <si>
+    <t>Side pr. Spørgsmål</t>
+  </si>
+  <si>
+    <t>Notifikationscheckbox</t>
+  </si>
+  <si>
+    <t>Burgeren kan vælge addresse v.h.a Google maps, når der oprettes en booking</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>Google maps addressen</t>
+  </si>
+  <si>
+    <t>UX3</t>
+  </si>
+  <si>
+    <t>UX1</t>
+  </si>
+  <si>
+    <t>UX2</t>
   </si>
 </sst>
 </file>
@@ -703,7 +733,7 @@
   <dimension ref="B2:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,28 +930,28 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
@@ -930,7 +960,7 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -952,100 +982,145 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>55</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
@@ -1149,12 +1224,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G20">
-    <sortCondition ref="F3:F20" customList="Skal,Burde,Kunne,Gerne"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G22">
+    <sortCondition ref="F3:F22" customList="Skal,Burde,Kunne,Gerne"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F19 F21:F36" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F36" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
       <formula1>"Skal,Burde,Kunne,Gerne,Hvis tid"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B17 B21:B36" xr:uid="{74B0885D-C444-4534-93C9-A891D8F15A37}">

</xml_diff>

<commit_message>
CRA, Move TestConstantsLib & update documentation
</commit_message>
<xml_diff>
--- a/Documents/CitizenTaxi.xlsx
+++ b/Documents/CitizenTaxi.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F03C94-1C4B-4D78-A64C-C2047849C209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A70F8D-248E-40EA-9170-16C1BC144190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
     <sheet name="Estimeret tidsplan" sheetId="4" r:id="rId2"/>
+    <sheet name="Realiseret tidsplan" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="104">
   <si>
     <t>Krav Id</t>
   </si>
@@ -416,12 +417,15 @@
   <si>
     <t>13/11 til 16/11</t>
   </si>
+  <si>
+    <t>Ja</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +443,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB17ED8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -482,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -697,11 +708,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,7 +749,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -745,12 +777,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -764,12 +792,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -779,6 +801,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,12 +828,12 @@
   <colors>
     <mruColors>
       <color rgb="FFD5B8EA"/>
+      <color rgb="FFB17ED8"/>
       <color rgb="FFF29E6A"/>
       <color rgb="FF000000"/>
       <color rgb="FFFFECAF"/>
       <color rgb="FF6C6A6A"/>
       <color rgb="FF575555"/>
-      <color rgb="FFB17ED8"/>
       <color rgb="FF9751CB"/>
       <color rgb="FFA365D1"/>
       <color rgb="FFB3DE7E"/>
@@ -1109,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922BD6CB-9F3E-455F-858E-49A0A21094EE}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1237,9 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="C6" t="s">
         <v>45</v>
       </c>
@@ -1215,7 +1257,9 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="C7" t="s">
         <v>46</v>
       </c>
@@ -1413,19 +1457,19 @@
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="33" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1622,7 +1666,7 @@
   <dimension ref="B1:AG14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,480 +1689,811 @@
     </row>
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="11">
+      <c r="C4" s="46"/>
+      <c r="D4" s="10">
         <v>45236</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>45237</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>45238</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>45239</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>45240</v>
       </c>
-      <c r="I4" s="15">
-        <v>45241</v>
-      </c>
-      <c r="J4" s="15">
-        <v>45242</v>
-      </c>
-      <c r="K4" s="15">
+      <c r="I4" s="14">
         <v>45243</v>
       </c>
-      <c r="L4" s="15">
+      <c r="J4" s="14">
         <v>45244</v>
       </c>
-      <c r="M4" s="15">
+      <c r="K4" s="14">
         <v>45245</v>
       </c>
-      <c r="N4" s="12">
+      <c r="L4" s="14">
         <v>45246</v>
       </c>
-      <c r="O4" s="12">
+      <c r="M4" s="14">
         <v>45247</v>
       </c>
-      <c r="P4" s="12">
-        <v>45248</v>
-      </c>
-      <c r="Q4" s="12">
-        <v>45249</v>
-      </c>
-      <c r="R4" s="12">
+      <c r="N4" s="11">
         <v>45250</v>
       </c>
-      <c r="S4" s="15">
+      <c r="O4" s="11">
         <v>45251</v>
       </c>
-      <c r="T4" s="15">
+      <c r="P4" s="11">
         <v>45252</v>
       </c>
-      <c r="U4" s="15">
+      <c r="Q4" s="11">
         <v>45253</v>
       </c>
-      <c r="V4" s="15">
+      <c r="R4" s="11">
         <v>45254</v>
       </c>
-      <c r="W4" s="15">
-        <v>45255</v>
-      </c>
-      <c r="X4" s="12">
-        <v>45256</v>
-      </c>
-      <c r="Y4" s="12">
+      <c r="S4" s="14">
         <v>45257</v>
       </c>
-      <c r="Z4" s="12">
+      <c r="T4" s="14">
         <v>45258</v>
       </c>
-      <c r="AA4" s="12">
+      <c r="U4" s="14">
         <v>45259</v>
       </c>
-      <c r="AB4" s="12">
+      <c r="V4" s="14">
         <v>45260</v>
       </c>
-      <c r="AC4" s="17">
+      <c r="W4" s="16">
         <v>45261</v>
       </c>
     </row>
     <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="S5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="U5" s="16" t="s">
+      <c r="U5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="V5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="W5" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="X5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y5" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z5" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA5" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB5" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC5" s="18" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="32"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="27"/>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="42"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
-      <c r="AC8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="24"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="22"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="31"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="26"/>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="29"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="24"/>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="26"/>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="24"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="26"/>
+    </row>
+    <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EB829-7EF3-4323-B00C-E54D52F1FFB2}">
+  <dimension ref="B1:AG14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+    </row>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="46"/>
+      <c r="D4" s="10">
+        <v>45236</v>
+      </c>
+      <c r="E4" s="11">
+        <v>45237</v>
+      </c>
+      <c r="F4" s="11">
+        <v>45238</v>
+      </c>
+      <c r="G4" s="11">
+        <v>45239</v>
+      </c>
+      <c r="H4" s="11">
+        <v>45240</v>
+      </c>
+      <c r="I4" s="14">
+        <v>45243</v>
+      </c>
+      <c r="J4" s="14">
+        <v>45244</v>
+      </c>
+      <c r="K4" s="14">
+        <v>45245</v>
+      </c>
+      <c r="L4" s="14">
+        <v>45246</v>
+      </c>
+      <c r="M4" s="14">
+        <v>45247</v>
+      </c>
+      <c r="N4" s="11">
+        <v>45250</v>
+      </c>
+      <c r="O4" s="11">
+        <v>45251</v>
+      </c>
+      <c r="P4" s="11">
+        <v>45252</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>45253</v>
+      </c>
+      <c r="R4" s="11">
+        <v>45254</v>
+      </c>
+      <c r="S4" s="14">
+        <v>45257</v>
+      </c>
+      <c r="T4" s="14">
+        <v>45258</v>
+      </c>
+      <c r="U4" s="14">
+        <v>45259</v>
+      </c>
+      <c r="V4" s="14">
+        <v>45260</v>
+      </c>
+      <c r="W4" s="16">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="27"/>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="42"/>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="24"/>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="26"/>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="24"/>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="31"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="26"/>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="29"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="24"/>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="31"/>
+      <c r="W13" s="26"/>
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
       <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Usabilitytest assignments + bug fixes and style updates
</commit_message>
<xml_diff>
--- a/Documents/CitizenTaxi.xlsx
+++ b/Documents/CitizenTaxi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2996DAB8-E4BA-44B6-B450-7C47E30F8F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7652E3-FD4F-4B9B-A1EC-FD73DFE55845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
   <si>
     <t>Krav Id</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Viderestilling efter login</t>
   </si>
   <si>
-    <t>Admin CRUD Patient</t>
-  </si>
-  <si>
     <t>Admin CRUD Notat</t>
   </si>
   <si>
@@ -419,6 +416,21 @@
   </si>
   <si>
     <t>Ja</t>
+  </si>
+  <si>
+    <t>lør</t>
+  </si>
+  <si>
+    <t>søn</t>
+  </si>
+  <si>
+    <t>Admin CRUD Borger</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
+  <si>
+    <t>Delvist</t>
   </si>
 </sst>
 </file>
@@ -810,13 +822,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922BD6CB-9F3E-455F-858E-49A0A21094EE}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,15 +1193,17 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -1199,15 +1213,17 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -1217,15 +1233,17 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -1236,90 +1254,96 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -1329,15 +1353,17 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
@@ -1347,51 +1373,57 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>5</v>
@@ -1401,50 +1433,57 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
@@ -1454,33 +1493,37 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+      <c r="B18" s="35" t="s">
+        <v>102</v>
+      </c>
       <c r="C18" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="35" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
@@ -1490,55 +1533,63 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" t="s">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1647,7 +1698,7 @@
     <sortCondition ref="F3:F22" customList="Skal,Burde,Kunne,Gerne"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F36" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
       <formula1>"Skal,Burde,Kunne,Gerne,Hvis tid"</formula1>
     </dataValidation>
@@ -1663,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EEC40F-AABE-47F4-AD1E-AF9E525F9CEA}">
   <dimension ref="B1:AG14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,10 +1738,10 @@
     </row>
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="46"/>
+      <c r="B4" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="47"/>
       <c r="D4" s="10">
         <v>45236</v>
       </c>
@@ -1754,78 +1805,78 @@
     </row>
     <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="H5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="N5" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="Q5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="R5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="T5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="U5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="W5" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="V5" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="W5" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="39"/>
@@ -1850,10 +1901,10 @@
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="36"/>
@@ -1878,10 +1929,10 @@
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="20"/>
@@ -1906,10 +1957,10 @@
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="22"/>
@@ -1934,10 +1985,10 @@
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="20"/>
@@ -1962,10 +2013,10 @@
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="22"/>
@@ -1990,10 +2041,10 @@
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="20"/>
@@ -2018,10 +2069,10 @@
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="22"/>
@@ -2046,10 +2097,10 @@
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -2084,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EB829-7EF3-4323-B00C-E54D52F1FFB2}">
   <dimension ref="B1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,10 +2159,10 @@
     </row>
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="46"/>
+      <c r="B4" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="47"/>
       <c r="D4" s="10">
         <v>45236</v>
       </c>
@@ -2157,96 +2208,108 @@
       <c r="R4" s="11">
         <v>45254</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="11">
+        <v>45255</v>
+      </c>
+      <c r="T4" s="11">
+        <v>45256</v>
+      </c>
+      <c r="U4" s="14">
         <v>45257</v>
       </c>
-      <c r="T4" s="14">
+      <c r="V4" s="14">
         <v>45258</v>
       </c>
-      <c r="U4" s="14">
+      <c r="W4" s="14">
         <v>45259</v>
       </c>
-      <c r="V4" s="14">
+      <c r="X4" s="14">
         <v>45260</v>
       </c>
-      <c r="W4" s="16">
+      <c r="Y4" s="16">
         <v>45261</v>
       </c>
     </row>
     <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="H5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="N5" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="Q5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="R5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="W5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="X5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y5" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="V5" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="W5" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="39"/>
@@ -2267,14 +2330,16 @@
       <c r="T6" s="19"/>
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
-      <c r="W6" s="27"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="27"/>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="36"/>
@@ -2293,16 +2358,18 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="42"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="42"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="20"/>
@@ -2323,14 +2390,16 @@
       <c r="T8" s="20"/>
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
-      <c r="W8" s="24"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="24"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="22"/>
@@ -2351,14 +2420,16 @@
       <c r="T9" s="22"/>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
-      <c r="W9" s="26"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="26"/>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="20"/>
@@ -2379,14 +2450,16 @@
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
-      <c r="W10" s="24"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="24"/>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="22"/>
@@ -2398,23 +2471,25 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
       <c r="T11" s="22"/>
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
-      <c r="W11" s="26"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="26"/>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="20"/>
@@ -2435,14 +2510,16 @@
       <c r="T12" s="20"/>
       <c r="U12" s="20"/>
       <c r="V12" s="20"/>
-      <c r="W12" s="24"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="24"/>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="22"/>
@@ -2460,38 +2537,42 @@
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
+      <c r="T13" s="18"/>
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
-      <c r="W13" s="26"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="26"/>
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
-      <c r="W14" s="9"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Most of product report
</commit_message>
<xml_diff>
--- a/Documents/CitizenTaxi.xlsx
+++ b/Documents/CitizenTaxi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7652E3-FD4F-4B9B-A1EC-FD73DFE55845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C9B18-7058-4A3E-827B-E35AE707667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-45105" yWindow="4665" windowWidth="16410" windowHeight="9645" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Brugernes kode skal enkrypteres før loginoplysningerne gemmes i databasen</t>
   </si>
   <si>
-    <t>Brugeren bliver omstillet til loginsiden</t>
-  </si>
-  <si>
     <t>Efter brugerlogin gemmes en token i cookies, som er med til at verificere brugerens identitet</t>
   </si>
   <si>
@@ -431,6 +428,9 @@
   </si>
   <si>
     <t>Delvist</t>
+  </si>
+  <si>
+    <t>Brugeren bliver omstillet til loginsiden, når de ikke er logget ind</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
   <dimension ref="B2:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,36 +1194,36 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -1234,16 +1234,16 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -1254,96 +1254,96 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -1354,16 +1354,16 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
@@ -1374,56 +1374,56 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>5</v>
@@ -1434,56 +1434,56 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
@@ -1494,102 +1494,102 @@
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="35" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
         <v>49</v>
-      </c>
-      <c r="G21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
     <sortCondition ref="F3:F22" customList="Skal,Burde,Kunne,Gerne"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F36" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
       <formula1>"Skal,Burde,Kunne,Gerne,Hvis tid"</formula1>
     </dataValidation>
@@ -1739,7 +1739,7 @@
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="10">
@@ -1805,78 +1805,78 @@
     </row>
     <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="H5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="N5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="Q5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="R5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="U5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="V5" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="W5" s="17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="39"/>
@@ -1901,10 +1901,10 @@
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="36"/>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="20"/>
@@ -1957,10 +1957,10 @@
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="22"/>
@@ -1985,10 +1985,10 @@
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="20"/>
@@ -2013,10 +2013,10 @@
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="22"/>
@@ -2041,10 +2041,10 @@
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="20"/>
@@ -2069,10 +2069,10 @@
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="22"/>
@@ -2097,10 +2097,10 @@
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -2136,7 +2136,7 @@
   <dimension ref="B1:AG14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2160,7 @@
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="10">
@@ -2232,84 +2232,84 @@
     </row>
     <row r="5" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="H5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="N5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="Q5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="R5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="V5" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="W5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="X5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y5" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="V5" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="X5" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y5" s="17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="39"/>
@@ -2336,10 +2336,10 @@
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="36"/>
@@ -2356,20 +2356,20 @@
       <c r="P7" s="41"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
       <c r="W7" s="40"/>
       <c r="X7" s="40"/>
       <c r="Y7" s="42"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="20"/>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="22"/>
@@ -2426,10 +2426,10 @@
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="20"/>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="22"/>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="20"/>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="22"/>
@@ -2538,7 +2538,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="18"/>
-      <c r="U13" s="22"/>
+      <c r="U13" s="18"/>
       <c r="V13" s="22"/>
       <c r="W13" s="22"/>
       <c r="X13" s="22"/>
@@ -2546,10 +2546,10 @@
     </row>
     <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -2566,8 +2566,8 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>

</xml_diff>

<commit_message>
Update timetable + process report
</commit_message>
<xml_diff>
--- a/Documents/CitizenTaxi.xlsx
+++ b/Documents/CitizenTaxi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\CitizenTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C9B18-7058-4A3E-827B-E35AE707667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A038860-B276-4624-8F4E-48D83FBB2A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45105" yWindow="4665" windowWidth="16410" windowHeight="9645" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-45120" yWindow="-4995" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922BD6CB-9F3E-455F-858E-49A0A21094EE}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EB829-7EF3-4323-B00C-E54D52F1FFB2}">
   <dimension ref="B1:AG14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2360,7 @@
       <c r="T7" s="41"/>
       <c r="U7" s="41"/>
       <c r="V7" s="41"/>
-      <c r="W7" s="40"/>
+      <c r="W7" s="41"/>
       <c r="X7" s="40"/>
       <c r="Y7" s="42"/>
     </row>
@@ -2388,9 +2388,9 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="24"/>
     </row>

</xml_diff>